<commit_message>
Updated the Prosper Cada Indicator resource
</commit_message>
<xml_diff>
--- a/resources/Prosper Canada Indicator import sheet 2016-10-26.xlsx
+++ b/resources/Prosper Canada Indicator import sheet 2016-10-26.xlsx
@@ -3592,7 +3592,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3626,12 +3626,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3677,7 +3671,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3902,16 +3896,7 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8933,10 +8918,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N128"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="E96" sqref="E96"/>
+      <selection pane="topRight" activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -10341,13 +10326,13 @@
       <c r="A76" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B76" s="77" t="s">
+      <c r="B76" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="C76" s="77" t="s">
+      <c r="C76" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="D76" s="78" t="s">
+      <c r="D76" s="6" t="s">
         <v>488</v>
       </c>
       <c r="E76" s="31" t="s">
@@ -10358,13 +10343,13 @@
       <c r="A77" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="B77" s="77" t="s">
+      <c r="B77" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="C77" s="77" t="s">
+      <c r="C77" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="D77" s="76" t="s">
+      <c r="D77" s="8" t="s">
         <v>295</v>
       </c>
       <c r="E77" s="31" t="s">
@@ -10375,13 +10360,13 @@
       <c r="A78" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B78" s="77" t="s">
+      <c r="B78" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="C78" s="77" t="s">
+      <c r="C78" s="35" t="s">
         <v>298</v>
       </c>
-      <c r="D78" s="76" t="s">
+      <c r="D78" s="8" t="s">
         <v>300</v>
       </c>
       <c r="E78" s="31" t="s">
@@ -10392,13 +10377,13 @@
       <c r="A79" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="B79" s="77" t="s">
+      <c r="B79" s="35" t="s">
         <v>305</v>
       </c>
-      <c r="C79" s="77" t="s">
+      <c r="C79" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="D79" s="79" t="s">
+      <c r="D79" s="76" t="s">
         <v>306</v>
       </c>
       <c r="E79" s="31" t="s">
@@ -10409,13 +10394,13 @@
       <c r="A80" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="B80" s="77" t="s">
+      <c r="B80" s="35" t="s">
         <v>310</v>
       </c>
-      <c r="C80" s="77" t="s">
+      <c r="C80" s="35" t="s">
         <v>309</v>
       </c>
-      <c r="D80" s="79" t="s">
+      <c r="D80" s="76" t="s">
         <v>311</v>
       </c>
       <c r="E80" s="31" t="s">
@@ -10426,13 +10411,13 @@
       <c r="A81" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="B81" s="77" t="s">
+      <c r="B81" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="C81" s="77" t="s">
+      <c r="C81" s="35" t="s">
         <v>314</v>
       </c>
-      <c r="D81" s="76" t="s">
+      <c r="D81" s="8" t="s">
         <v>316</v>
       </c>
       <c r="E81" s="31" t="s">
@@ -10443,13 +10428,13 @@
       <c r="A82" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="B82" s="77" t="s">
+      <c r="B82" s="35" t="s">
         <v>320</v>
       </c>
-      <c r="C82" s="77" t="s">
+      <c r="C82" s="35" t="s">
         <v>319</v>
       </c>
-      <c r="D82" s="78" t="s">
+      <c r="D82" s="6" t="s">
         <v>321</v>
       </c>
       <c r="E82" s="31" t="s">
@@ -10460,13 +10445,13 @@
       <c r="A83" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B83" s="77" t="s">
+      <c r="B83" s="35" t="s">
         <v>325</v>
       </c>
-      <c r="C83" s="77" t="s">
+      <c r="C83" s="35" t="s">
         <v>324</v>
       </c>
-      <c r="D83" s="78" t="s">
+      <c r="D83" s="6" t="s">
         <v>326</v>
       </c>
       <c r="E83" s="31" t="s">
@@ -10477,13 +10462,13 @@
       <c r="A84" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="B84" s="77" t="s">
+      <c r="B84" s="35" t="s">
         <v>330</v>
       </c>
-      <c r="C84" s="77" t="s">
+      <c r="C84" s="35" t="s">
         <v>329</v>
       </c>
-      <c r="D84" s="78" t="s">
+      <c r="D84" s="6" t="s">
         <v>328</v>
       </c>
       <c r="E84" s="31" t="s">
@@ -10494,13 +10479,13 @@
       <c r="A85" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="B85" s="77" t="s">
+      <c r="B85" s="35" t="s">
         <v>334</v>
       </c>
-      <c r="C85" s="77" t="s">
+      <c r="C85" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="D85" s="78" t="s">
+      <c r="D85" s="6" t="s">
         <v>335</v>
       </c>
       <c r="E85" s="31" t="s">
@@ -10511,13 +10496,13 @@
       <c r="A86" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="B86" s="77" t="s">
+      <c r="B86" s="35" t="s">
         <v>339</v>
       </c>
-      <c r="C86" s="77" t="s">
+      <c r="C86" s="35" t="s">
         <v>338</v>
       </c>
-      <c r="D86" s="78" t="s">
+      <c r="D86" s="6" t="s">
         <v>340</v>
       </c>
       <c r="E86" s="31" t="s">
@@ -10528,13 +10513,13 @@
       <c r="A87" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="B87" s="77" t="s">
+      <c r="B87" s="35" t="s">
         <v>344</v>
       </c>
-      <c r="C87" s="77" t="s">
+      <c r="C87" s="35" t="s">
         <v>343</v>
       </c>
-      <c r="D87" s="78" t="s">
+      <c r="D87" s="6" t="s">
         <v>342</v>
       </c>
       <c r="E87" s="31" t="s">
@@ -10545,13 +10530,13 @@
       <c r="A88" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="B88" s="77" t="s">
+      <c r="B88" s="35" t="s">
         <v>348</v>
       </c>
-      <c r="C88" s="77" t="s">
+      <c r="C88" s="35" t="s">
         <v>347</v>
       </c>
-      <c r="D88" s="78" t="s">
+      <c r="D88" s="6" t="s">
         <v>349</v>
       </c>
       <c r="E88" s="31" t="s">
@@ -10562,13 +10547,13 @@
       <c r="A89" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="B89" s="77" t="s">
+      <c r="B89" s="35" t="s">
         <v>353</v>
       </c>
-      <c r="C89" s="77" t="s">
+      <c r="C89" s="35" t="s">
         <v>352</v>
       </c>
-      <c r="D89" s="78" t="s">
+      <c r="D89" s="6" t="s">
         <v>351</v>
       </c>
       <c r="E89" s="31" t="s">
@@ -10579,13 +10564,13 @@
       <c r="A90" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="B90" s="77" t="s">
+      <c r="B90" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="C90" s="77" t="s">
+      <c r="C90" s="35" t="s">
         <v>356</v>
       </c>
-      <c r="D90" s="78" t="s">
+      <c r="D90" s="6" t="s">
         <v>358</v>
       </c>
       <c r="E90" s="31" t="s">
@@ -10596,13 +10581,13 @@
       <c r="A91" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="B91" s="77" t="s">
+      <c r="B91" s="35" t="s">
         <v>362</v>
       </c>
-      <c r="C91" s="77" t="s">
+      <c r="C91" s="35" t="s">
         <v>361</v>
       </c>
-      <c r="D91" s="78" t="s">
+      <c r="D91" s="6" t="s">
         <v>363</v>
       </c>
       <c r="E91" s="31" t="s">
@@ -10613,13 +10598,13 @@
       <c r="A92" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="B92" s="77" t="s">
+      <c r="B92" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="C92" s="77" t="s">
+      <c r="C92" s="35" t="s">
         <v>366</v>
       </c>
-      <c r="D92" s="78" t="s">
+      <c r="D92" s="6" t="s">
         <v>368</v>
       </c>
       <c r="E92" s="31" t="s">
@@ -10630,13 +10615,13 @@
       <c r="A93" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="B93" s="77" t="s">
+      <c r="B93" s="35" t="s">
         <v>372</v>
       </c>
-      <c r="C93" s="77" t="s">
+      <c r="C93" s="35" t="s">
         <v>371</v>
       </c>
-      <c r="D93" s="78" t="s">
+      <c r="D93" s="6" t="s">
         <v>373</v>
       </c>
       <c r="E93" s="31" t="s">
@@ -10647,13 +10632,13 @@
       <c r="A94" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="B94" s="77" t="s">
+      <c r="B94" s="35" t="s">
         <v>377</v>
       </c>
-      <c r="C94" s="77" t="s">
+      <c r="C94" s="35" t="s">
         <v>376</v>
       </c>
-      <c r="D94" s="78" t="s">
+      <c r="D94" s="6" t="s">
         <v>378</v>
       </c>
       <c r="E94" s="31" t="s">
@@ -10664,13 +10649,13 @@
       <c r="A95" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="B95" s="77" t="s">
+      <c r="B95" s="35" t="s">
         <v>382</v>
       </c>
-      <c r="C95" s="77" t="s">
+      <c r="C95" s="35" t="s">
         <v>381</v>
       </c>
-      <c r="D95" s="78" t="s">
+      <c r="D95" s="6" t="s">
         <v>383</v>
       </c>
       <c r="E95" s="31" t="s">
@@ -10678,16 +10663,16 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="38.6" x14ac:dyDescent="0.4">
-      <c r="A96" s="78" t="s">
+      <c r="A96" s="6" t="s">
         <v>966</v>
       </c>
-      <c r="B96" s="77" t="s">
+      <c r="B96" s="35" t="s">
         <v>972</v>
       </c>
-      <c r="C96" s="77" t="s">
+      <c r="C96" s="35" t="s">
         <v>968</v>
       </c>
-      <c r="D96" s="78" t="s">
+      <c r="D96" s="6" t="s">
         <v>967</v>
       </c>
       <c r="E96" s="31" t="s">
@@ -13370,41 +13355,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A42:A48"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A56:A63"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="A72:A76"/>
-    <mergeCell ref="A78:A85"/>
-    <mergeCell ref="A87:A89"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A101:A105"/>
-    <mergeCell ref="A107:A111"/>
-    <mergeCell ref="A113:A117"/>
-    <mergeCell ref="A119:A122"/>
-    <mergeCell ref="A124:A129"/>
-    <mergeCell ref="A131:A136"/>
-    <mergeCell ref="A138:A143"/>
-    <mergeCell ref="A145:A155"/>
-    <mergeCell ref="A157:A159"/>
-    <mergeCell ref="A161:A163"/>
-    <mergeCell ref="A165:A167"/>
-    <mergeCell ref="A169:A171"/>
-    <mergeCell ref="A173:A175"/>
-    <mergeCell ref="A177:A179"/>
-    <mergeCell ref="A181:A183"/>
-    <mergeCell ref="A189:A191"/>
-    <mergeCell ref="A193:A195"/>
     <mergeCell ref="A217:A219"/>
     <mergeCell ref="A221:A223"/>
     <mergeCell ref="A225:A229"/>
@@ -13414,6 +13364,41 @@
     <mergeCell ref="A205:A207"/>
     <mergeCell ref="A209:A211"/>
     <mergeCell ref="A213:A215"/>
+    <mergeCell ref="A173:A175"/>
+    <mergeCell ref="A177:A179"/>
+    <mergeCell ref="A181:A183"/>
+    <mergeCell ref="A189:A191"/>
+    <mergeCell ref="A193:A195"/>
+    <mergeCell ref="A145:A155"/>
+    <mergeCell ref="A157:A159"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="A165:A167"/>
+    <mergeCell ref="A169:A171"/>
+    <mergeCell ref="A113:A117"/>
+    <mergeCell ref="A119:A122"/>
+    <mergeCell ref="A124:A129"/>
+    <mergeCell ref="A131:A136"/>
+    <mergeCell ref="A138:A143"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A101:A105"/>
+    <mergeCell ref="A107:A111"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A56:A63"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="A72:A76"/>
+    <mergeCell ref="A78:A85"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13695,17 +13680,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F88062E4732ABB44AAF0DDBD4DB7AEC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18dc41c3923c662a5725df878a8274e3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ff1b691-2d87-4848-a84d-7e4eb2cf7d7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f5a5027fc013b294d570711a07c07b3" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F88062E4732ABB44AAF0DDBD4DB7AEC6" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7bdbec071906a7b55b6ee46b062cfe9a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ff1b691-2d87-4848-a84d-7e4eb2cf7d7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c8087244fd7c3cf2e82bb7457ba10cd0" ns2:_="">
     <xsd:import namespace="9ff1b691-2d87-4848-a84d-7e4eb2cf7d7d"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -13852,21 +13834,32 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F11481-CEA2-42CE-ABBC-70B8A619D5A7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{629A990F-C23D-4012-B0DD-3E393E1EAFD7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9ff1b691-2d87-4848-a84d-7e4eb2cf7d7d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{073901FE-A781-4A84-B7DE-19E3C64D3DFB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{175BB9B5-9329-429A-9C3D-EAEF1586D61A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -13884,17 +13877,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{629A990F-C23D-4012-B0DD-3E393E1EAFD7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F11481-CEA2-42CE-ABBC-70B8A619D5A7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9ff1b691-2d87-4848-a84d-7e4eb2cf7d7d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>